<commit_message>
fix: ajusta layout, botões e inclui produtos e serviços
</commit_message>
<xml_diff>
--- a/backend/excel/ambientes.xlsx
+++ b/backend/excel/ambientes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,272 +424,323 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>cor_principal</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>ativo</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>nicho</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>nicho_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>modulos_habilitados</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>nome</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>logo_url</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>nome_empresa</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
         <is>
           <t>payment_status</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>plan</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>slug</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
         <is>
           <t>excel_file</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>modulos_habilitados</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>slug</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>nicho</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>nome</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>ativo</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>nicho_id</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>cor_principal</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>logo_url</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>nome_empresa</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>plan</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>#61d402</t>
+        </is>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Nutricionista</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Nutricionista</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>046fd9a3-ff2a-4ebd-90b8-ff94da3f2c86</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>["clientes", "equipe", "financeiro", "assinaturas", "dashboard"]</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Nutricionista Fernanda</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Nutricionista Fernanda</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nutri-fernanda</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
         <is>
           <t>nutri-fernanda.xlsx</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>["clientes", "equipe", "financeiro", "assinaturas", "dashboard"]</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nutri-fernanda</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Nutricionista</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Nutricionista Fernanda</t>
-        </is>
-      </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Nutricionista</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>#61d402</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Nutricionista Fernanda</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>#000000</t>
+        </is>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Advogado</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>8e643421-f9b5-4059-b8ec-11868bb2ba76</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Advogado Alisson</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>trial</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>enterprise</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>adv-alisson</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
         <is>
           <t>adv-alisson.xlsx</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>adv-alisson</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Advogado</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Advogado Alisson</t>
-        </is>
-      </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>#000000</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>enterprise</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>#6b90ff</t>
+        </is>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Educação</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>06c550a0-145c-4930-a970-b34564a7fa81</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Cassia Professora</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
         <is>
           <t>trial</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>enterprise</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>cassia-prof</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
         <is>
           <t>cassia-prof.xlsx</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>cassia-prof</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Educação</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Cassia Professora</t>
-        </is>
-      </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>#6b90ff</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>enterprise</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>#000000</t>
+        </is>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>f975d01d-cb6e-4528-8a0c-ba1f1fe640d0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>f975d01d-cb6e-4528-8a0c-ba1f1fe640d0</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>9505d0d3-8610-42fa-854d-5456810d1c02</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>["dashboard", "agenda", "produtos", "clientes", "assinaturas", "financeiro", "equipe", "leads_pipeline"]</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Barbearia Alpha</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>/static/logos/barb-alpha_234e5ec9.png</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Barbearia Alpha</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
         <is>
           <t>paid</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>enterprise</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>barb-alpha</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
         <is>
           <t>barb-alpha.xlsx</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>["dashboard", "agenda", "produtos", "clientes", "assinaturas", "financeiro", "equipe", "leads_pipeline"]</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>barb-alpha</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>#d4af37</t>
+        </is>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>f975d01d-cb6e-4528-8a0c-ba1f1fe640d0</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Barbearia Alpha</t>
-        </is>
-      </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>f975d01d-cb6e-4528-8a0c-ba1f1fe640d0</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>#000000</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>/static/logos/barb-alpha_234e5ec9.png</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Barbearia Alpha</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>27965b1e-edea-4c3d-8d3b-737a7294a1f1</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>["dashboard", "leads_pipeline", "agenda", "clientes", "equipe", "financeiro", "produtos", "assinaturas"]</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Barbearia do Janderson</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
         <is>
           <t>enterprise</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>barb-janderson</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>barb-janderson.xlsx</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Sistema de notificações Toast, redefinição de senha, e melhorias visuais
- Criado ToastContext.jsx com sistema de notificações elegantes
- Adicionado toast.css com estilos premium para notificações
- Implementado funcionalidade de redefinir senha no Profile.jsx
- Adicionados estilos btn-icon, btn-icon-danger, btn-icon-settings e btn-close-modal
- Corrigido contraste da lista de Configurações Ativas no modal de nichos
- Melhorado tratamento de erros com mensagens amigáveis
- Reposicionado botão de engrenagem para canto superior direito dos cards
- Substituídos todos os alert() por toast elegantes
</commit_message>
<xml_diff>
--- a/backend/excel/ambientes.xlsx
+++ b/backend/excel/ambientes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,323 +424,327 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>cnpj</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nicho</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>contract_status</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>logo_url</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>plan</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>payment_status</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>nome</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>excel_file</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>slug</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>contract_signed_url</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>modulos_habilitados</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>nome_empresa</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>ativo</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
           <t>cor_principal</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>ativo</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>nicho</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>contract_generated_url</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>endereco</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
         <is>
           <t>nicho_id</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>modulos_habilitados</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>nome</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>logo_url</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>nome_empresa</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>payment_status</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>plan</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>slug</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>excel_file</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>#61d402</t>
-        </is>
-      </c>
-      <c r="B2" t="b">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>f975d01d-cb6e-4528-8a0c-ba1f1fe640d0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>signed</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>/static/logos/barb-alpha_234e5ec9.png</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>enterprise</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>paid</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Barbearia Alpha</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>barb-alpha.xlsx</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>barb-alpha</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>storage\barb-alpha\contrato_assinado_7cfc7d.pdf</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>["dashboard", "agenda", "produtos", "clientes", "assinaturas", "financeiro", "equipe", "leads_pipeline", "ai_agent"]</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Barbearia Alpha</t>
+        </is>
+      </c>
+      <c r="M2" t="b">
         <v>1</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Nutricionista</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Nutricionista</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>046fd9a3-ff2a-4ebd-90b8-ff94da3f2c86</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>["clientes", "equipe", "financeiro", "assinaturas", "dashboard"]</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Nutricionista Fernanda</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Nutricionista Fernanda</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nutri-fernanda</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nutri-fernanda.xlsx</t>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>#000000</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>storage\barb-alpha\contrato_ambiente_barb-alpha.pdf</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>f975d01d-cb6e-4528-8a0c-ba1f1fe640d0</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>9505d0d3-8610-42fa-854d-5456810d1c02</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>#000000</t>
-        </is>
-      </c>
-      <c r="B3" t="b">
-        <v>1</v>
+          <t>123456789000175</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Advogado</t>
+          <t>signed</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>/static/logos/barb-jp_8265bcab.png</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>8e643421-f9b5-4059-b8ec-11868bb2ba76</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Advogado Alisson</t>
+          <t>pro</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>barb-jp.xlsx</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>barb-jp</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>trial</t>
+          <t>storage\barb-jp\contrato_assinado_022226.pdf</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>enterprise</t>
+          <t>["dashboard", "leads_pipeline", "agenda", "clientes", "equipe", "financeiro", "financeiro", "produtos", "assinaturas", "ai_agent"]</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>adv-alisson</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>adv-alisson.xlsx</t>
+          <t>Barbearia JP</t>
+        </is>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>#d4af37</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>storage\barb-jp\contrato_ambiente_barb-jp.pdf</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>JOSE DELMIRO DOS SANTOS, 409</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>f975d01d-cb6e-4528-8a0c-ba1f1fe640d0</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>0dfb2838-61d1-468b-bea1-c00ea4f464b4</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>#6b90ff</t>
-        </is>
-      </c>
-      <c r="B4" t="b">
-        <v>1</v>
+          <t>13385063000163</t>
+        </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Educação</t>
+          <t>generated</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>/static/logos/barb-antonio_dc7747a2.png</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>06c550a0-145c-4930-a970-b34564a7fa81</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Cassia Professora</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
+          <t>pro</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>trial</t>
         </is>
       </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>barb-antonio.xlsx</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>barb-antonio</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>enterprise</t>
+          <t>["dashboard", "leads_pipeline", "agenda", "clientes", "equipe", "financeiro", "financeiro", "produtos", "assinaturas", "ai_agent"]</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>cassia-prof</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>cassia-prof.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>#000000</t>
-        </is>
-      </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" t="inlineStr">
+          <t>Barbearia Antonio</t>
+        </is>
+      </c>
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>#d4af37</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>storage\barb-antonio\contrato_ambiente_barb-antonio.pdf</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Rua Caetés 342</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
         <is>
           <t>f975d01d-cb6e-4528-8a0c-ba1f1fe640d0</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>f975d01d-cb6e-4528-8a0c-ba1f1fe640d0</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>9505d0d3-8610-42fa-854d-5456810d1c02</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>["dashboard", "agenda", "produtos", "clientes", "assinaturas", "financeiro", "equipe", "leads_pipeline"]</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Barbearia Alpha</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>/static/logos/barb-alpha_234e5ec9.png</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Barbearia Alpha</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>paid</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>enterprise</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>barb-alpha</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>barb-alpha.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>#d4af37</t>
-        </is>
-      </c>
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>f975d01d-cb6e-4528-8a0c-ba1f1fe640d0</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>27965b1e-edea-4c3d-8d3b-737a7294a1f1</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>["dashboard", "leads_pipeline", "agenda", "clientes", "equipe", "financeiro", "produtos", "assinaturas"]</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Barbearia do Janderson</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>trial</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>enterprise</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>barb-janderson</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>barb-janderson.xlsx</t>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>10d4673c-cd1d-4094-b354-720aef978282</t>
         </is>
       </c>
     </row>

</xml_diff>